<commit_message>
I think these was some clean up? ...
</commit_message>
<xml_diff>
--- a/output/article/Supp-mat4_model_diets_10000.xlsx
+++ b/output/article/Supp-mat4_model_diets_10000.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="159">
   <si>
     <t xml:space="preserve">Code_sp</t>
   </si>
@@ -74,9 +74,6 @@
     <t xml:space="preserve">other_sp_code</t>
   </si>
   <si>
-    <t xml:space="preserve">mean_diet</t>
-  </si>
-  <si>
     <t xml:space="preserve">Eco_area</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t xml:space="preserve">no</t>
   </si>
   <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
     <t xml:space="preserve">Bera_bai</t>
   </si>
   <si>
@@ -108,9 +102,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ohizumi et al 2003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.1906595329766, 0, 0, 0, 53.1076553827691, 0, 0.295014750737537, 33.4066703335167, 0, 0, 0, 0, 0</t>
   </si>
   <si>
     <t xml:space="preserve">Bala_bon</t>
@@ -915,16 +906,13 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
       </c>
       <c r="C2" t="n">
         <v>4.94079361446792</v>
@@ -966,67 +954,87 @@
         <v>9.22049340674184</v>
       </c>
       <c r="P2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" t="s">
         <v>25</v>
       </c>
-      <c r="R2" t="s">
-        <v>26</v>
-      </c>
       <c r="S2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T2"/>
-      <c r="U2" t="s">
-        <v>28</v>
-      </c>
-      <c r="V2"/>
+      <c r="U2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="n">
+        <v>13.1906595329766</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>53.1076553827691</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.295014750737537</v>
+      </c>
+      <c r="J3" t="n">
+        <v>33.4066703335167</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3" t="s">
-        <v>31</v>
-      </c>
       <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" t="s">
         <v>25</v>
       </c>
-      <c r="R3" t="s">
-        <v>26</v>
-      </c>
       <c r="S3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T3"/>
-      <c r="U3" t="s">
-        <v>32</v>
-      </c>
-      <c r="V3"/>
+      <c r="U3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -1068,31 +1076,28 @@
         <v>95</v>
       </c>
       <c r="P4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Q4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="S4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T4"/>
       <c r="U4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -1134,31 +1139,28 @@
         <v>100</v>
       </c>
       <c r="P5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="Q5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="S5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T5"/>
       <c r="U5" t="s">
-        <v>28</v>
-      </c>
-      <c r="V5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -1200,31 +1202,28 @@
         <v>10</v>
       </c>
       <c r="P6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="Q6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="S6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T6"/>
       <c r="U6" t="s">
-        <v>28</v>
-      </c>
-      <c r="V6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -1266,31 +1265,28 @@
         <v>100</v>
       </c>
       <c r="P7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="Q7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="S7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T7"/>
       <c r="U7" t="s">
-        <v>28</v>
-      </c>
-      <c r="V7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -1332,31 +1328,28 @@
         <v>100</v>
       </c>
       <c r="P8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="S8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T8"/>
       <c r="U8" t="s">
-        <v>28</v>
-      </c>
-      <c r="V8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -1398,29 +1391,26 @@
         <v>100</v>
       </c>
       <c r="P9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Q9" t="s">
+        <v>24</v>
+      </c>
+      <c r="R9" t="s">
         <v>25</v>
       </c>
-      <c r="R9" t="s">
-        <v>26</v>
-      </c>
       <c r="S9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T9"/>
-      <c r="U9" t="s">
-        <v>28</v>
-      </c>
-      <c r="V9"/>
+      <c r="U9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -1462,29 +1452,26 @@
         <v>0</v>
       </c>
       <c r="P10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q10" t="s">
+        <v>24</v>
+      </c>
+      <c r="R10" t="s">
         <v>25</v>
       </c>
-      <c r="R10" t="s">
-        <v>26</v>
-      </c>
       <c r="S10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T10"/>
-      <c r="U10" t="s">
-        <v>28</v>
-      </c>
-      <c r="V10"/>
+      <c r="U10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C11" t="n">
         <v>4.85532271431529</v>
@@ -1526,29 +1513,26 @@
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="Q11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="R11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T11"/>
-      <c r="U11" t="s">
-        <v>28</v>
-      </c>
-      <c r="V11"/>
+      <c r="U11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C12" t="n">
         <v>3.70741482965932</v>
@@ -1590,29 +1574,26 @@
         <v>0</v>
       </c>
       <c r="P12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="R12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T12"/>
-      <c r="U12" t="s">
-        <v>28</v>
-      </c>
-      <c r="V12"/>
+      <c r="U12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C13" t="n">
         <v>1.16974972796518</v>
@@ -1654,31 +1635,28 @@
         <v>0</v>
       </c>
       <c r="P13" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>24</v>
+      </c>
+      <c r="R13" t="s">
+        <v>62</v>
+      </c>
+      <c r="S13" t="s">
+        <v>63</v>
+      </c>
+      <c r="T13" t="s">
         <v>64</v>
       </c>
-      <c r="Q13" t="s">
-        <v>25</v>
-      </c>
-      <c r="R13" t="s">
-        <v>65</v>
-      </c>
-      <c r="S13" t="s">
-        <v>66</v>
-      </c>
-      <c r="T13" t="s">
-        <v>67</v>
-      </c>
-      <c r="U13" t="s">
-        <v>28</v>
-      </c>
-      <c r="V13"/>
+      <c r="U13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -1720,31 +1698,28 @@
         <v>0</v>
       </c>
       <c r="P14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="Q14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="S14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T14"/>
       <c r="U14" t="s">
-        <v>28</v>
-      </c>
-      <c r="V14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C15" t="n">
         <v>1.16974972796518</v>
@@ -1786,29 +1761,26 @@
         <v>0</v>
       </c>
       <c r="P15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Q15" t="s">
+        <v>24</v>
+      </c>
+      <c r="R15" t="s">
         <v>25</v>
       </c>
-      <c r="R15" t="s">
-        <v>26</v>
-      </c>
       <c r="S15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T15"/>
-      <c r="U15" t="s">
-        <v>28</v>
-      </c>
-      <c r="V15"/>
+      <c r="U15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C16" t="n">
         <v>0.217974513749162</v>
@@ -1850,29 +1822,26 @@
         <v>0</v>
       </c>
       <c r="P16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="Q16" t="s">
+        <v>24</v>
+      </c>
+      <c r="R16" t="s">
         <v>25</v>
       </c>
-      <c r="R16" t="s">
-        <v>26</v>
-      </c>
       <c r="S16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T16"/>
-      <c r="U16" t="s">
-        <v>28</v>
-      </c>
-      <c r="V16"/>
+      <c r="U16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -1914,29 +1883,26 @@
         <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="Q17" t="s">
+        <v>24</v>
+      </c>
+      <c r="R17" t="s">
         <v>25</v>
       </c>
-      <c r="R17" t="s">
-        <v>26</v>
-      </c>
       <c r="S17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T17"/>
-      <c r="U17" t="s">
-        <v>28</v>
-      </c>
-      <c r="V17"/>
+      <c r="U17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -1978,31 +1944,28 @@
         <v>0</v>
       </c>
       <c r="P18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Q18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="S18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T18" t="s">
-        <v>83</v>
-      </c>
-      <c r="U18" t="s">
-        <v>28</v>
-      </c>
-      <c r="V18"/>
+        <v>80</v>
+      </c>
+      <c r="U18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C19" t="n">
         <v>0.108279193736465</v>
@@ -2044,29 +2007,26 @@
         <v>0</v>
       </c>
       <c r="P19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="Q19" t="s">
+        <v>24</v>
+      </c>
+      <c r="R19" t="s">
         <v>25</v>
       </c>
-      <c r="R19" t="s">
-        <v>26</v>
-      </c>
       <c r="S19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T19"/>
-      <c r="U19" t="s">
-        <v>28</v>
-      </c>
-      <c r="V19"/>
+      <c r="U19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C20" t="n">
         <v>16.0518444666002</v>
@@ -2108,29 +2068,26 @@
         <v>0</v>
       </c>
       <c r="P20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="Q20" t="s">
+        <v>24</v>
+      </c>
+      <c r="R20" t="s">
         <v>25</v>
       </c>
-      <c r="R20" t="s">
-        <v>26</v>
-      </c>
       <c r="S20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T20"/>
-      <c r="U20" t="s">
-        <v>28</v>
-      </c>
-      <c r="V20"/>
+      <c r="U20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C21" t="n">
         <v>94.1585631718962</v>
@@ -2172,29 +2129,26 @@
         <v>0</v>
       </c>
       <c r="P21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q21" t="s">
+        <v>24</v>
+      </c>
+      <c r="R21" t="s">
         <v>25</v>
       </c>
-      <c r="R21" t="s">
-        <v>26</v>
-      </c>
       <c r="S21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T21"/>
-      <c r="U21" t="s">
-        <v>28</v>
-      </c>
-      <c r="V21"/>
+      <c r="U21"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C22" t="n">
         <v>5</v>
@@ -2236,31 +2190,28 @@
         <v>0</v>
       </c>
       <c r="P22" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="Q22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="S22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T22"/>
       <c r="U22" t="s">
-        <v>28</v>
-      </c>
-      <c r="V22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -2302,31 +2253,28 @@
         <v>0</v>
       </c>
       <c r="P23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="Q23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R23" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="S23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T23"/>
       <c r="U23" t="s">
-        <v>28</v>
-      </c>
-      <c r="V23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C24" t="n">
         <v>23.3</v>
@@ -2368,29 +2316,26 @@
         <v>0</v>
       </c>
       <c r="P24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Q24" t="s">
+        <v>24</v>
+      </c>
+      <c r="R24" t="s">
         <v>25</v>
       </c>
-      <c r="R24" t="s">
-        <v>26</v>
-      </c>
       <c r="S24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T24"/>
-      <c r="U24" t="s">
-        <v>28</v>
-      </c>
-      <c r="V24"/>
+      <c r="U24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C25" t="n">
         <v>2.40211322433545</v>
@@ -2432,29 +2377,26 @@
         <v>0</v>
       </c>
       <c r="P25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="Q25" t="s">
+        <v>24</v>
+      </c>
+      <c r="R25" t="s">
         <v>25</v>
       </c>
-      <c r="R25" t="s">
-        <v>26</v>
-      </c>
       <c r="S25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T25"/>
-      <c r="U25" t="s">
-        <v>28</v>
-      </c>
-      <c r="V25"/>
+      <c r="U25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
@@ -2496,31 +2438,28 @@
         <v>50</v>
       </c>
       <c r="P26" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="Q26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="S26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T26"/>
       <c r="U26" t="s">
-        <v>28</v>
-      </c>
-      <c r="V26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B27" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C27" t="n">
         <v>20</v>
@@ -2562,31 +2501,28 @@
         <v>0</v>
       </c>
       <c r="P27" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="Q27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="S27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T27"/>
       <c r="U27" t="s">
-        <v>28</v>
-      </c>
-      <c r="V27" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B28" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
@@ -2628,29 +2564,26 @@
         <v>0</v>
       </c>
       <c r="P28" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="Q28" t="s">
+        <v>24</v>
+      </c>
+      <c r="R28" t="s">
         <v>25</v>
       </c>
-      <c r="R28" t="s">
-        <v>26</v>
-      </c>
       <c r="S28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T28"/>
-      <c r="U28" t="s">
-        <v>28</v>
-      </c>
-      <c r="V28"/>
+      <c r="U28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C29" t="n">
         <v>15.4699648246862</v>
@@ -2692,29 +2625,26 @@
         <v>0</v>
       </c>
       <c r="P29" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Q29" t="s">
+        <v>24</v>
+      </c>
+      <c r="R29" t="s">
         <v>25</v>
       </c>
-      <c r="R29" t="s">
-        <v>26</v>
-      </c>
       <c r="S29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T29"/>
-      <c r="U29" t="s">
-        <v>28</v>
-      </c>
-      <c r="V29"/>
+      <c r="U29"/>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B30" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
@@ -2756,29 +2686,26 @@
         <v>0</v>
       </c>
       <c r="P30" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="Q30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R30" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="S30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T30"/>
-      <c r="U30" t="s">
-        <v>28</v>
-      </c>
-      <c r="V30"/>
+      <c r="U30"/>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B31" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C31" t="n">
         <v>0.155123380540634</v>
@@ -2820,29 +2747,26 @@
         <v>0</v>
       </c>
       <c r="P31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="Q31" t="s">
+        <v>24</v>
+      </c>
+      <c r="R31" t="s">
         <v>25</v>
       </c>
-      <c r="R31" t="s">
-        <v>26</v>
-      </c>
       <c r="S31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T31"/>
-      <c r="U31" t="s">
-        <v>28</v>
-      </c>
-      <c r="V31"/>
+      <c r="U31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C32" t="n">
         <v>32.5926130381576</v>
@@ -2884,29 +2808,26 @@
         <v>0.0499500499500499</v>
       </c>
       <c r="P32" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="Q32" t="s">
+        <v>24</v>
+      </c>
+      <c r="R32" t="s">
         <v>25</v>
       </c>
-      <c r="R32" t="s">
-        <v>26</v>
-      </c>
       <c r="S32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T32"/>
-      <c r="U32" t="s">
-        <v>28</v>
-      </c>
-      <c r="V32"/>
+      <c r="U32"/>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
@@ -2948,29 +2869,26 @@
         <v>0</v>
       </c>
       <c r="P33" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Q33" t="s">
+        <v>24</v>
+      </c>
+      <c r="R33" t="s">
         <v>25</v>
       </c>
-      <c r="R33" t="s">
-        <v>26</v>
-      </c>
       <c r="S33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T33"/>
-      <c r="U33" t="s">
-        <v>28</v>
-      </c>
-      <c r="V33"/>
+      <c r="U33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B34" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -3012,31 +2930,28 @@
         <v>0</v>
       </c>
       <c r="P34" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="Q34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="S34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T34"/>
       <c r="U34" t="s">
-        <v>28</v>
-      </c>
-      <c r="V34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C35" t="n">
         <v>12.572862909612</v>
@@ -3078,31 +2993,28 @@
         <v>0</v>
       </c>
       <c r="P35" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="Q35" t="s">
+        <v>24</v>
+      </c>
+      <c r="R35" t="s">
         <v>25</v>
       </c>
-      <c r="R35" t="s">
-        <v>26</v>
-      </c>
       <c r="S35" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="T35" t="s">
-        <v>138</v>
-      </c>
-      <c r="U35" t="s">
-        <v>28</v>
-      </c>
-      <c r="V35"/>
+        <v>135</v>
+      </c>
+      <c r="U35"/>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B36" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C36" t="n">
         <v>18.7836264952673</v>
@@ -3144,29 +3056,26 @@
         <v>0</v>
       </c>
       <c r="P36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="Q36" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="R36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T36"/>
-      <c r="U36" t="s">
-        <v>28</v>
-      </c>
-      <c r="V36"/>
+      <c r="U36"/>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B37" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -3208,29 +3117,26 @@
         <v>0</v>
       </c>
       <c r="P37" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="Q37" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="R37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T37"/>
-      <c r="U37" t="s">
-        <v>28</v>
-      </c>
-      <c r="V37"/>
+      <c r="U37"/>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B38" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C38" t="n">
         <v>6.46298981615747</v>
@@ -3272,29 +3178,26 @@
         <v>0</v>
       </c>
       <c r="P38" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="Q38" t="s">
+        <v>24</v>
+      </c>
+      <c r="R38" t="s">
         <v>25</v>
       </c>
-      <c r="R38" t="s">
-        <v>26</v>
-      </c>
       <c r="S38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T38"/>
-      <c r="U38" t="s">
-        <v>28</v>
-      </c>
-      <c r="V38"/>
+      <c r="U38"/>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B39" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
@@ -3336,31 +3239,28 @@
         <v>0</v>
       </c>
       <c r="P39" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="Q39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R39" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="S39" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T39" t="s">
-        <v>128</v>
-      </c>
-      <c r="U39" t="s">
-        <v>28</v>
-      </c>
-      <c r="V39"/>
+        <v>125</v>
+      </c>
+      <c r="U39"/>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B40" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C40" t="n">
         <v>66.0277353780005</v>
@@ -3402,31 +3302,28 @@
         <v>0</v>
       </c>
       <c r="P40" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="Q40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R40" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="S40" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T40" t="s">
-        <v>154</v>
-      </c>
-      <c r="U40" t="s">
-        <v>28</v>
-      </c>
-      <c r="V40"/>
+        <v>151</v>
+      </c>
+      <c r="U40"/>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B41" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C41" t="n">
         <v>42.2042872056484</v>
@@ -3468,29 +3365,26 @@
         <v>0</v>
       </c>
       <c r="P41" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Q41" t="s">
+        <v>24</v>
+      </c>
+      <c r="R41" t="s">
         <v>25</v>
       </c>
-      <c r="R41" t="s">
-        <v>26</v>
-      </c>
       <c r="S41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T41"/>
-      <c r="U41" t="s">
-        <v>28</v>
-      </c>
-      <c r="V41"/>
+      <c r="U41"/>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B42" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C42" t="n">
         <v>66.0277353780005</v>
@@ -3532,29 +3426,26 @@
         <v>0</v>
       </c>
       <c r="P42" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="Q42" t="s">
+        <v>24</v>
+      </c>
+      <c r="R42" t="s">
         <v>25</v>
       </c>
-      <c r="R42" t="s">
-        <v>26</v>
-      </c>
       <c r="S42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T42"/>
-      <c r="U42" t="s">
-        <v>28</v>
-      </c>
-      <c r="V42"/>
+      <c r="U42"/>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B43" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -3596,22 +3487,19 @@
         <v>0</v>
       </c>
       <c r="P43" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="Q43" t="s">
+        <v>24</v>
+      </c>
+      <c r="R43" t="s">
         <v>25</v>
       </c>
-      <c r="R43" t="s">
-        <v>26</v>
-      </c>
       <c r="S43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T43"/>
-      <c r="U43" t="s">
-        <v>28</v>
-      </c>
-      <c r="V43"/>
+      <c r="U43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>